<commit_message>
chore: contamination, delete segmented models, replace by spearman's tests => PAH
</commit_message>
<xml_diff>
--- a/inst/results/data_contam/PAH/summarised_levels_data_PAH_dw.xlsx
+++ b/inst/results/data_contam/PAH/summarised_levels_data_PAH_dw.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -351,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,196 +361,301 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>ESTUARY</t>
+          <t>PARAMETRE_LIBELLE</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>PARAMETRE_LIBELLE</t>
+          <t>First 5 years</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>median_ng_gdw</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>median_1</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>median_2</t>
+          <t>Last 5 years</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Gironde</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Anthracène</t>
-        </is>
+          <t>Anthracene</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>1.05</v>
       </c>
       <c r="C2">
-        <v>1.5645</v>
-      </c>
-      <c r="D2">
-        <v>0.3448</v>
-      </c>
-      <c r="E2">
-        <v>0.5395</v>
+        <v>1.53</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Loire</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Anthracène</t>
-        </is>
+          <t>Benzo-anthra.</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>6.1</v>
       </c>
       <c r="C3">
-        <v>0.694</v>
-      </c>
-      <c r="D3">
-        <v>0.1724</v>
-      </c>
-      <c r="E3">
-        <v>0.2393</v>
+        <v>3.6305</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Seine</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Anthracène</t>
-        </is>
+          <t>Benzo-peryl.</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>7.6</v>
       </c>
       <c r="C4">
-        <v>2.517</v>
-      </c>
-      <c r="D4">
-        <v>0.7413999999999999</v>
-      </c>
-      <c r="E4">
-        <v>0.8679</v>
+        <v>5.179</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Gironde</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Benzo(a)anthracène</t>
-        </is>
+          <t>Benzo-pyr.</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>1.5</v>
       </c>
       <c r="C5">
-        <v>3.172</v>
-      </c>
-      <c r="D5">
-        <v>5.312</v>
-      </c>
-      <c r="E5">
-        <v>3.965</v>
+        <v>2.3895</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Loire</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Benzo(a)anthracène</t>
-        </is>
+          <t>Fluoranthene</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>27</v>
       </c>
       <c r="C6">
-        <v>2.936</v>
-      </c>
-      <c r="D6">
-        <v>5.125</v>
-      </c>
-      <c r="E6">
-        <v>3.67</v>
+        <v>10.674</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Seine</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Benzo(a)anthracène</t>
-        </is>
+          <t>Naphtalene</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>16</v>
       </c>
       <c r="C7">
-        <v>13.021</v>
-      </c>
-      <c r="D7">
-        <v>23.44</v>
-      </c>
-      <c r="E7">
-        <v>16.28</v>
+        <v>0.571</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Gironde</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Benzo(a)pyrène</t>
-        </is>
+          <t>Phenanthrene</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>15</v>
       </c>
       <c r="C8">
-        <v>1.7345</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0.2891</v>
+        <v>7.101</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>Pyrene</t>
+        </is>
+      </c>
+      <c r="B9">
+        <v>15.5</v>
+      </c>
+      <c r="C9">
+        <v>9.877000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ESTUARY</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>PARAMETRE_LIBELLE</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>First 5 years</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Last 5 years</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Gironde</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Anthracene</t>
+        </is>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1.5645</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>Loire</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Anthracene</t>
+        </is>
+      </c>
+      <c r="C3">
+        <v>0.5</v>
+      </c>
+      <c r="D3">
+        <v>0.694</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Seine</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Anthracene</t>
+        </is>
+      </c>
+      <c r="C4">
+        <v>2.15</v>
+      </c>
+      <c r="D4">
+        <v>2.517</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Gironde</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Benzo-anthra.</t>
+        </is>
+      </c>
+      <c r="C5">
+        <v>4.25</v>
+      </c>
+      <c r="D5">
+        <v>3.172</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Loire</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Benzo-anthra.</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>4.1</v>
+      </c>
+      <c r="D6">
+        <v>2.936</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Seine</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Benzo-anthra.</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>18.75</v>
+      </c>
+      <c r="D7">
+        <v>13.021</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Gironde</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Benzo-peryl.</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>3.3</v>
+      </c>
+      <c r="D8">
+        <v>5.3105</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Loire</t>
+        </is>
+      </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Benzo(a)pyrène</t>
+          <t>Benzo-peryl.</t>
         </is>
       </c>
       <c r="C9">
-        <v>1.655</v>
+        <v>5.85</v>
       </c>
       <c r="D9">
-        <v>0.0625</v>
-      </c>
-      <c r="E9">
-        <v>0.2758</v>
+        <v>4.297499999999999</v>
       </c>
     </row>
     <row r="10">
@@ -560,17 +666,14 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Benzo(a)pyrène</t>
+          <t>Benzo-peryl.</t>
         </is>
       </c>
       <c r="C10">
-        <v>8.776</v>
+        <v>15.5</v>
       </c>
       <c r="D10">
-        <v>0.5583</v>
-      </c>
-      <c r="E10">
-        <v>1.463</v>
+        <v>14.41</v>
       </c>
     </row>
     <row r="11">
@@ -581,17 +684,14 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Benzo(g,h,i)pérylène</t>
+          <t>Benzo-pyr.</t>
         </is>
       </c>
       <c r="C11">
-        <v>5.3105</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>3</v>
-      </c>
-      <c r="E11">
-        <v>4.828</v>
+        <v>1.7345</v>
       </c>
     </row>
     <row r="12">
@@ -602,17 +702,14 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Benzo(g,h,i)pérylène</t>
+          <t>Benzo-pyr.</t>
         </is>
       </c>
       <c r="C12">
-        <v>4.297499999999999</v>
+        <v>0.375</v>
       </c>
       <c r="D12">
-        <v>5.318</v>
-      </c>
-      <c r="E12">
-        <v>3.907</v>
+        <v>1.655</v>
       </c>
     </row>
     <row r="13">
@@ -623,17 +720,14 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Benzo(g,h,i)pérylène</t>
+          <t>Benzo-pyr.</t>
         </is>
       </c>
       <c r="C13">
-        <v>14.41</v>
+        <v>3.35</v>
       </c>
       <c r="D13">
-        <v>14.09</v>
-      </c>
-      <c r="E13">
-        <v>13.1</v>
+        <v>8.776</v>
       </c>
     </row>
     <row r="14">
@@ -644,17 +738,14 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Fluoranthène</t>
+          <t>Fluoranthene</t>
         </is>
       </c>
       <c r="C14">
+        <v>10.5</v>
+      </c>
+      <c r="D14">
         <v>9.073499999999999</v>
-      </c>
-      <c r="D14">
-        <v>9.545</v>
-      </c>
-      <c r="E14">
-        <v>8.249000000000001</v>
       </c>
     </row>
     <row r="15">
@@ -665,17 +756,14 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Fluoranthène</t>
+          <t>Fluoranthene</t>
         </is>
       </c>
       <c r="C15">
+        <v>18</v>
+      </c>
+      <c r="D15">
         <v>8.435500000000001</v>
-      </c>
-      <c r="D15">
-        <v>16.36</v>
-      </c>
-      <c r="E15">
-        <v>7.669</v>
       </c>
     </row>
     <row r="16">
@@ -686,17 +774,14 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Fluoranthène</t>
+          <t>Fluoranthene</t>
         </is>
       </c>
       <c r="C16">
+        <v>58</v>
+      </c>
+      <c r="D16">
         <v>25.704</v>
-      </c>
-      <c r="D16">
-        <v>52.73</v>
-      </c>
-      <c r="E16">
-        <v>23.37</v>
       </c>
     </row>
     <row r="17">
@@ -707,16 +792,13 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Naphtalène</t>
+          <t>Naphtalene</t>
         </is>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>54.5</v>
       </c>
       <c r="D17">
-        <v>16.03</v>
-      </c>
-      <c r="E17">
         <v>0</v>
       </c>
     </row>
@@ -728,17 +810,14 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Naphtalène</t>
+          <t>Naphtalene</t>
         </is>
       </c>
       <c r="C18">
+        <v>14</v>
+      </c>
+      <c r="D18">
         <v>0.747</v>
-      </c>
-      <c r="D18">
-        <v>4.118</v>
-      </c>
-      <c r="E18">
-        <v>0.2197</v>
       </c>
     </row>
     <row r="19">
@@ -749,17 +828,14 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Naphtalène</t>
+          <t>Naphtalene</t>
         </is>
       </c>
       <c r="C19">
+        <v>18</v>
+      </c>
+      <c r="D19">
         <v>0.5449999999999999</v>
-      </c>
-      <c r="D19">
-        <v>5.294</v>
-      </c>
-      <c r="E19">
-        <v>0.1603</v>
       </c>
     </row>
     <row r="20">
@@ -770,17 +846,14 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Phénanthrène</t>
+          <t>Phenanthrene</t>
         </is>
       </c>
       <c r="C20">
+        <v>7.4</v>
+      </c>
+      <c r="D20">
         <v>5.5705</v>
-      </c>
-      <c r="D20">
-        <v>0.4353</v>
-      </c>
-      <c r="E20">
-        <v>0.3277</v>
       </c>
     </row>
     <row r="21">
@@ -791,17 +864,14 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Phénanthrène</t>
+          <t>Phenanthrene</t>
         </is>
       </c>
       <c r="C21">
+        <v>16</v>
+      </c>
+      <c r="D21">
         <v>7.047499999999999</v>
-      </c>
-      <c r="D21">
-        <v>0.9412</v>
-      </c>
-      <c r="E21">
-        <v>0.4146</v>
       </c>
     </row>
     <row r="22">
@@ -812,17 +882,14 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Phénanthrène</t>
+          <t>Phenanthrene</t>
         </is>
       </c>
       <c r="C22">
+        <v>27.25</v>
+      </c>
+      <c r="D22">
         <v>8.81</v>
-      </c>
-      <c r="D22">
-        <v>1.603</v>
-      </c>
-      <c r="E22">
-        <v>0.5182</v>
       </c>
     </row>
     <row r="23">
@@ -833,17 +900,14 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Pyrène</t>
+          <t>Pyrene</t>
         </is>
       </c>
       <c r="C23">
+        <v>10.05</v>
+      </c>
+      <c r="D23">
         <v>9.640499999999999</v>
-      </c>
-      <c r="D23">
-        <v>10.05</v>
-      </c>
-      <c r="E23">
-        <v>9.640000000000001</v>
       </c>
     </row>
     <row r="24">
@@ -854,17 +918,14 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Pyrène</t>
+          <t>Pyrene</t>
         </is>
       </c>
       <c r="C24">
+        <v>12.25</v>
+      </c>
+      <c r="D24">
         <v>8.649000000000001</v>
-      </c>
-      <c r="D24">
-        <v>12.25</v>
-      </c>
-      <c r="E24">
-        <v>8.648999999999999</v>
       </c>
     </row>
     <row r="25">
@@ -875,16 +936,13 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Pyrène</t>
+          <t>Pyrene</t>
         </is>
       </c>
       <c r="C25">
-        <v>28</v>
+        <v>53.25</v>
       </c>
       <c r="D25">
-        <v>53.25</v>
-      </c>
-      <c r="E25">
         <v>28</v>
       </c>
     </row>

</xml_diff>